<commit_message>
Solution fixed so Dictionary is built everytime
Dictionary:
- Beautified Dictionary.ico a bit
- Made the word coloring based on the types
- Shortcuts for Add, Edit, Delete and Translate buttons
Added some tasks into LanguageToolsTasks.xlsx
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks and Bugs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Project</t>
   </si>
@@ -40,10 +40,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t xml:space="preserve">Automatically switch to SQL Repository, so I don't need to go switch manually. Create a config file where the last preference is stored
-</t>
-  </si>
-  <si>
     <t>Have sort by type of the word</t>
   </si>
   <si>
@@ -51,13 +47,57 @@
   </si>
   <si>
     <t>Progress %</t>
+  </si>
+  <si>
+    <t>Automatically switch to SQL Repository, so I don't need to go switch manually. Create a config file where the last preference is stored</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you try to change the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>word type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on SQL Repository it won't work. It is changed localy but not propagated to the databade.</t>
+    </r>
+  </si>
+  <si>
+    <t>Create and Edit Languague</t>
+  </si>
+  <si>
+    <t>Color the words based on the type in various languages</t>
+  </si>
+  <si>
+    <t>Ability to turn on/off the coloring</t>
+  </si>
+  <si>
+    <t>Present user with a keyboard with the letters of the current language. This should be available as an option.</t>
+  </si>
+  <si>
+    <t>Recolor the word if the wordtype changes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +108,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -410,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +486,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -458,7 +506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -467,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -478,20 +526,20 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A22" si="0">A3+1</f>
+        <f t="shared" ref="A4:A25" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -503,118 +551,209 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>A5+0.1</f>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>A6+0.1</f>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f>A7+0.1</f>
+        <v>4.2999999999999989</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
+      <c r="E10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a Keyboard as a separate window (Windows.Forms)
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -461,7 +461,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Keyboard Window: increased the height of the button to 35 to accomodate Spanish ñ - LanguageWindow for adding and editing languages (only xml repository support) - Repository: AddLanguage return bool: true if succesfully added a new Language
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Project</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Recolor the word if the wordtype changes</t>
+  </si>
+  <si>
+    <t>Works for English only</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Only XMLRepository</t>
   </si>
 </sst>
 </file>
@@ -458,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,9 +479,10 @@
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="73.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -488,8 +498,11 @@
       <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -506,7 +519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -524,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A25" si="0">A3+1</f>
         <v>3</v>
@@ -542,7 +555,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -560,7 +573,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+0.1</f>
         <v>4.0999999999999996</v>
@@ -575,10 +588,13 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6+0.1</f>
         <v>4.1999999999999993</v>
@@ -596,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>A7+0.1</f>
         <v>4.2999999999999989</v>
@@ -614,7 +630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>A5+1</f>
         <v>5</v>
@@ -632,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -650,7 +666,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -665,34 +681,37 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>12</v>

</xml_diff>

<commit_message>
- Refactored switch between repositories: settings file contain preferences of repositories where the first entry is default - Removed unused methods
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +534,7 @@
         <v>7</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Some clean-ups and refactoring - TransliterationEditor: Filter rules and exapmles based on textboxes - TransliterationEditor: Fixed dashes option which was broken - UI testing for Dictionary - still not testint anything yet - Transliteration Algorithm takes into account counterexamples such that a rule is not applicable for them
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
   <si>
     <t>Project</t>
   </si>
@@ -100,6 +100,69 @@
   </si>
   <si>
     <t>Only XMLRepository</t>
+  </si>
+  <si>
+    <t>needs testing</t>
+  </si>
+  <si>
+    <t>DictionaryTest</t>
+  </si>
+  <si>
+    <t>Create UI testing project with some tests</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>DictionaryAndroid</t>
+  </si>
+  <si>
+    <t>DictionaryIPhone</t>
+  </si>
+  <si>
+    <t>Create an Android project for Dictionary</t>
+  </si>
+  <si>
+    <t>Create an iPhone project for Dictionary</t>
+  </si>
+  <si>
+    <t>TransliterationEditor</t>
+  </si>
+  <si>
+    <t>Count on number of rules and count on number of examples</t>
+  </si>
+  <si>
+    <t>Create a backup of the Dictionary SQL databade</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Transliterator</t>
+  </si>
+  <si>
+    <t>Make the algorithm take into account the CounterExamples such that the rule is not applicable for them</t>
+  </si>
+  <si>
+    <t>Make search for rules</t>
+  </si>
+  <si>
+    <t>Make search for examples</t>
+  </si>
+  <si>
+    <t>TransliteraitonEditor</t>
+  </si>
+  <si>
+    <t>Button "Reload and retest" should reload counter examples as they affect transliteraiton now</t>
+  </si>
+  <si>
+    <t>Deutsch: Sharp s and double s replace each other in the DB, so they can't coexist.</t>
+  </si>
+  <si>
+    <t>Deleting examples crashes the app</t>
+  </si>
+  <si>
+    <t>In examples introduce "distance" column which measures expected to transliterated distance</t>
   </si>
 </sst>
 </file>
@@ -469,14 +532,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="73.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" customWidth="1"/>
@@ -516,7 +579,10 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -692,80 +758,221 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>21</v>

</xml_diff>

<commit_message>
- German sharp s handled in SqlRepository - Some clean-ups - LanguageToolsTasks updated
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
         <v>7</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,7 +963,7 @@
         <v>7</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Tests: redone DB tests for some language combinations whit Serbian as destination, some refactoring - TransliterationEditor: showing distance between expected and transliterated - TransliterationEditor: fixed "Reload Languages"
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +768,7 @@
         <v>24</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -786,7 +786,7 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>7</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Fixed some bugs - Introduced category("Long") for tests
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>Project</t>
   </si>
@@ -129,9 +129,6 @@
     <t>TransliterationEditor</t>
   </si>
   <si>
-    <t>Count on number of rules and count on number of examples</t>
-  </si>
-  <si>
     <t>Create a backup of the Dictionary SQL databade</t>
   </si>
   <si>
@@ -163,6 +160,15 @@
   </si>
   <si>
     <t>In examples introduce "distance" column which measures expected to transliterated distance</t>
+  </si>
+  <si>
+    <t>Add Icon</t>
+  </si>
+  <si>
+    <t>Adding rule or example with (') crashes the application</t>
+  </si>
+  <si>
+    <t>Count on number of rules, count on number of examples, total distance</t>
   </si>
 </sst>
 </file>
@@ -532,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +822,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -831,10 +837,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
         <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -846,10 +852,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -867,7 +873,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -885,7 +891,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -900,10 +906,10 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -918,10 +924,10 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -939,13 +945,13 @@
         <v>29</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -954,10 +960,10 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -971,11 +977,35 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First update to 4.5.2 developer pack from http://www.microsoft.com/en-us/download/confirmation.aspx?id=42637 - Some projects updated to 4.5.2 (those that don't affect the web application Transliteration) - TransliterationEditor: Added a nice icoon from shell32.dll - Added tests for Transliteraiton from Serbian to German, English, Spanish and Russian
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
- Dictionary: rule for checking for language name relaxed a bit to allow "Hrvatski/Srpski latinica" - Dictionary: fixed managing the word types - adding and removing now works with SQL
</commit_message>
<xml_diff>
--- a/LanguageToolsTasks.xlsx
+++ b/LanguageToolsTasks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>Project</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Count on number of rules, count on number of examples, total distance</t>
+  </si>
+  <si>
+    <t>DATABASE</t>
   </si>
 </sst>
 </file>
@@ -538,14 +541,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="3" max="3" width="73.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" customWidth="1"/>
@@ -836,6 +839,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>